<commit_message>
& - 22268 от 06.10.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Croatia/#EURO#Croatia#Commemorative#[2023-present]#UNC.xlsx
+++ b/Collections/EURO/Croatia/#EURO#Croatia#Commemorative#[2023-present]#UNC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Croatia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C26E79-D68B-4648-B019-F9702674895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCE5344-DEAA-4B41-AEEC-91072793B6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4170" yWindow="1430" windowWidth="33150" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -81,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -171,6 +174,12 @@
   </si>
   <si>
     <t>Subtype_2#Special_marks_1</t>
+  </si>
+  <si>
+    <t>1100th Anniversary - Kingdom of Croatia and the Coronation of King Tomislav</t>
+  </si>
+  <si>
+    <t>400.000</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,23 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -533,9 +558,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -810,7 +835,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -944,7 +969,9 @@
       <c r="A6" s="5">
         <v>2025</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
         <v>18</v>
@@ -952,9 +979,11 @@
       <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="9" t="str">
         <f>IF(OR(AND(G6&gt;1,G6&lt;&gt;"-")),"Can exchange","")</f>
@@ -994,7 +1023,7 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1011,7 +1040,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1028,7 +1057,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G7))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1045,7 +1074,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G5))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>